<commit_message>
asynchronious calls with excel data ok
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
     <t xml:space="preserve">textType</t>
   </si>
   <si>
-    <t xml:space="preserve">author</t>
+    <t xml:space="preserve">Ville Vinha</t>
   </si>
   <si>
     <t xml:space="preserve">kirja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ville Vinha</t>
   </si>
   <si>
     <t xml:space="preserve">Keimo Kurvi</t>
@@ -162,18 +162,18 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up upload response
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="8">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">lehti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mikko Mallikas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keke Amstrong</t>
   </si>
 </sst>
 </file>
@@ -111,8 +117,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -133,10 +143,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -176,6 +186,374 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
first test of embedded publications
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -20,24 +20,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t xml:space="preserve">author</t>
   </si>
   <si>
-    <t xml:space="preserve">arvosana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uusi kenttä</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kille k.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hyvö</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erikoinen</t>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publish location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reception type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minna canth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Työmiehen vaimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workman’s wife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finnish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tampere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toinen teos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hella Wuolijoki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hassu näytelmä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a funny play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helsinki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gunilla Svensson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobbarens fru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swedish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stockholm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alle gulle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aslkdjasd alsdk j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alskjd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd</t>
   </si>
 </sst>
 </file>
@@ -119,12 +215,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -134,15 +230,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -155,16 +253,193 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1890</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1899</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1940</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1866</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1866</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FInally a working uploader function
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -122,18 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">alle gulle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aslkdjasd alsdk j</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alskjd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asd</t>
   </si>
 </sst>
 </file>
@@ -230,10 +218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,22 +414,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixed get enpoint for a single publication
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -58,6 +58,12 @@
     <t xml:space="preserve">reception type</t>
   </si>
   <si>
+    <t xml:space="preserve">Publication name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author type</t>
+  </si>
+  <si>
     <t xml:space="preserve">minna canth</t>
   </si>
   <si>
@@ -121,7 +127,52 @@
     <t xml:space="preserve">translation</t>
   </si>
   <si>
-    <t xml:space="preserve">alle gulle</t>
+    <t xml:space="preserve">Lisa Andersson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiina Toimittaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uskomattoman hassu kokemus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an unbelieveably funny experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">journal article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">news</t>
+  </si>
+  <si>
+    <t xml:space="preserve">review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virpi Virtanen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hieno teos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a fine work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venla Virtanen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vielä hienompi teos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">an even finer work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natalija Ivanova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">замечательное произведение</t>
   </si>
 </sst>
 </file>
@@ -131,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -152,6 +203,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,8 +254,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,200 +280,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>1890</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1899</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1940</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1866</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1866</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1950</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1989</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add delete metod for all authors
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -64,6 +64,15 @@
     <t xml:space="preserve">author type</t>
   </si>
   <si>
+    <t xml:space="preserve">publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link</t>
+  </si>
+  <si>
     <t xml:space="preserve">minna canth</t>
   </si>
   <si>
@@ -173,6 +182,27 @@
   </si>
   <si>
     <t xml:space="preserve">замечательное произведение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jotuni Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Новинки финской драматургии привезли в Петербург театральные деятели страны Суоми</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uutinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТАСС – Санкт-Петербург</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://aafnet.integrum.ru.libproxy.tuni.fi/artefact3/ia/ia5.aspx?lv=6&amp;si=jGVfDEFV2E&amp;qu=231&amp;st=0&amp;bi=5699&amp;xi=&amp;nd=1&amp;tnd=0&amp;srt=0&amp;f=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">творчество современных драматургов востребовано театрами Финляндии, которые помогают писателям, создающим произведения для театра, в их творческом становлении. В таком живом контакте создавались пьесы "Бесчувственность" Пиркко Сайсио и "Золотой телец" Марии Йотуни, посвященные проблемам современного общества.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -211,6 +241,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,7 +267,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,8 +291,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,15 +304,84 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -280,20 +390,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
@@ -342,263 +452,301 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>1890</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1899</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1940</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1866</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="G6" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1866</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1950</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1989</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1999</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="N13" s="2" t="n">
+        <v>38685</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R13" s="0"/>
+      <c r="S13" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>